<commit_message>
Integrated Selenium GRID with AFW
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EAB53C-9040-46D4-B836-3AF24B63A653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E34AE4-66BE-48E7-AF1B-BC2D77259B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>manager</t>
   </si>
@@ -27,6 +28,12 @@
   </si>
   <si>
     <t>ADMIN</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -401,10 +408,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A34F9BD-9479-4992-AD8F-93BA20667F4C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>